<commit_message>
changed filenames and added more exercises
</commit_message>
<xml_diff>
--- a/exercises.xlsx
+++ b/exercises.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="6555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>https://leetcode.com/problems/decode-ways/</t>
   </si>
   <si>
-    <t>decode ways</t>
-  </si>
-  <si>
     <t>recursive</t>
   </si>
   <si>
@@ -41,18 +38,12 @@
     <t>dfs</t>
   </si>
   <si>
-    <t>two sum</t>
-  </si>
-  <si>
     <t>array</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/two-sum/</t>
   </si>
   <si>
-    <t>valid parentheses</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/valid-parentheses/</t>
   </si>
   <si>
@@ -60,6 +51,114 @@
   </si>
   <si>
     <t>stack</t>
+  </si>
+  <si>
+    <t>linked list</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>two pointers</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/invert-binary-tree/</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>recursion</t>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-search/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-anagram/</t>
+  </si>
+  <si>
+    <t>binary search</t>
+  </si>
+  <si>
+    <t>Flood Fill</t>
+  </si>
+  <si>
+    <t>Valid Parentheses</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Decode Ways</t>
+  </si>
+  <si>
+    <t>matrix</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flood-fill/</t>
+  </si>
+  <si>
+    <t>bfs</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of a Binary Tree</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/balanced-binary-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle/</t>
+  </si>
+  <si>
+    <t>Linked list cycle</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-queue-using-stacks/</t>
+  </si>
+  <si>
+    <t>Implement Queue using Stacks</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/first-bad-version/</t>
+  </si>
+  <si>
+    <t>First Bad Version</t>
   </si>
 </sst>
 </file>
@@ -110,12 +209,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -397,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,16 +512,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -427,38 +529,214 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added problems till kclosest points to origin
</commit_message>
<xml_diff>
--- a/exercises.xlsx
+++ b/exercises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
   <si>
     <t>https://leetcode.com/problems/decode-ways/</t>
   </si>
@@ -134,9 +134,6 @@
     <t>https://leetcode.com/problems/balanced-binary-tree/</t>
   </si>
   <si>
-    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/linked-list-cycle/</t>
   </si>
   <si>
@@ -159,6 +156,87 @@
   </si>
   <si>
     <t>First Bad Version</t>
+  </si>
+  <si>
+    <t>Ransom Note</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/ransom-note/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/climbing-stairs/</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>dynamic programing</t>
+  </si>
+  <si>
+    <t>Longest palindrome</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-palindrome/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element/</t>
+  </si>
+  <si>
+    <t>Majority Element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-binary/</t>
+  </si>
+  <si>
+    <t>Add Binary</t>
+  </si>
+  <si>
+    <t>binary math</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/diameter-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>Diameter of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/middle-of-the-linked-list/</t>
+  </si>
+  <si>
+    <t>Middle of the Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/contains-duplicate/</t>
+  </si>
+  <si>
+    <t>Contains Duplicate</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray/</t>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-interval/</t>
+  </si>
+  <si>
+    <t>Insert Interval</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/01-matrix/</t>
+  </si>
+  <si>
+    <t>01 matrix</t>
   </si>
 </sst>
 </file>
@@ -499,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,8 +730,8 @@
       <c r="D10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>36</v>
+      <c r="E10" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -675,7 +753,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -684,23 +762,23 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -709,12 +787,12 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -723,7 +801,169 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -735,8 +975,9 @@
     <hyperlink ref="E7" r:id="rId5"/>
     <hyperlink ref="E8" r:id="rId6"/>
     <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="E10" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 3sum, longest substring and documented kclosest and balanced tree
</commit_message>
<xml_diff>
--- a/exercises.xlsx
+++ b/exercises.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="6480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="3735"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
   <si>
     <t>https://leetcode.com/problems/decode-ways/</t>
   </si>
@@ -237,6 +237,27 @@
   </si>
   <si>
     <t>01 matrix</t>
+  </si>
+  <si>
+    <t>longest substring without repeating characters</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/</t>
+  </si>
+  <si>
+    <t>k closest points to origin</t>
+  </si>
+  <si>
+    <t>heap</t>
+  </si>
+  <si>
+    <t>3sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/3sum/</t>
+  </si>
+  <si>
+    <t>arrray</t>
   </si>
 </sst>
 </file>
@@ -577,15 +598,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -964,6 +985,45 @@
       </c>
       <c r="E27" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
binary tree, clone graph, course schedule and rpn
</commit_message>
<xml_diff>
--- a/exercises.xlsx
+++ b/exercises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t>https://leetcode.com/problems/decode-ways/</t>
   </si>
@@ -258,6 +258,39 @@
   </si>
   <si>
     <t>arrray</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal/</t>
+  </si>
+  <si>
+    <t>binary tree level order traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/k-closest-points-to-origin/</t>
+  </si>
+  <si>
+    <t>clone graph</t>
+  </si>
+  <si>
+    <t>dict of node references</t>
+  </si>
+  <si>
+    <t>bfs or dfs</t>
+  </si>
+  <si>
+    <t>evaluate reverse polish notation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/clone-graph</t>
+  </si>
+  <si>
+    <t>course schedule</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/course-schedule/</t>
   </si>
 </sst>
 </file>
@@ -598,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,6 +1030,9 @@
       <c r="C28" t="s">
         <v>74</v>
       </c>
+      <c r="E28" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1024,6 +1060,65 @@
       </c>
       <c r="E30" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
7 more exercises from blind75
</commit_message>
<xml_diff>
--- a/exercises.xlsx
+++ b/exercises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="107">
   <si>
     <t>https://leetcode.com/problems/decode-ways/</t>
   </si>
@@ -291,6 +291,60 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>implement trie prefix tree</t>
+  </si>
+  <si>
+    <t>dict of dicts</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-trie-prefix-tree/</t>
+  </si>
+  <si>
+    <t>coin change</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/coin-change</t>
+  </si>
+  <si>
+    <t>dynamic programming</t>
+  </si>
+  <si>
+    <t>product of array except self</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/product-of-array-except-self/</t>
+  </si>
+  <si>
+    <t>cum prod</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/min-stack/</t>
+  </si>
+  <si>
+    <t>min stack</t>
+  </si>
+  <si>
+    <t>two stacks</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/validate-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>number of islands</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-islands/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotting-oranges/</t>
+  </si>
+  <si>
+    <t>validate binary search tree</t>
+  </si>
+  <si>
+    <t>rotting oranges</t>
   </si>
 </sst>
 </file>
@@ -631,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +696,7 @@
     <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -655,11 +709,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -669,11 +723,11 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -683,22 +737,22 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -708,11 +762,11 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -722,11 +776,11 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -736,11 +790,11 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -750,11 +804,11 @@
       <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -767,11 +821,11 @@
       <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -784,11 +838,11 @@
       <c r="D10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -801,11 +855,11 @@
       <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -815,22 +869,22 @@
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -840,11 +894,11 @@
       <c r="C14" t="s">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -854,11 +908,11 @@
       <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -868,11 +922,11 @@
       <c r="C16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -882,11 +936,11 @@
       <c r="C17" t="s">
         <v>48</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -896,11 +950,11 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -910,22 +964,22 @@
       <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
       <c r="B20" t="s">
         <v>55</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -938,11 +992,11 @@
       <c r="D21" t="s">
         <v>3</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -952,11 +1006,11 @@
       <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -966,44 +1020,44 @@
       <c r="C23" t="s">
         <v>3</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>64</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>68</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -1016,11 +1070,11 @@
       <c r="D27" t="s">
         <v>32</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -1030,11 +1084,11 @@
       <c r="C28" t="s">
         <v>74</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -1044,11 +1098,11 @@
       <c r="C29" t="s">
         <v>4</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -1058,11 +1112,11 @@
       <c r="C30" t="s">
         <v>12</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -1075,11 +1129,11 @@
       <c r="D31" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -1092,19 +1146,22 @@
       <c r="D32" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>84</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -1117,22 +1174,137 @@
       <c r="D34" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" t="s">
+        <v>100</v>
+      </c>
+      <c r="F38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40">
+        <v>24</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
-    <hyperlink ref="E9" r:id="rId7"/>
-    <hyperlink ref="E10" r:id="rId8"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F4" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F9" r:id="rId7"/>
+    <hyperlink ref="F10" r:id="rId8"/>
+    <hyperlink ref="F36" r:id="rId9"/>
+    <hyperlink ref="F40" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merge intervals, combination sum, permutations and search in rotated sorted array
</commit_message>
<xml_diff>
--- a/exercises.xlsx
+++ b/exercises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="118">
   <si>
     <t>https://leetcode.com/problems/decode-ways/</t>
   </si>
@@ -257,9 +257,6 @@
     <t>https://leetcode.com/problems/3sum/</t>
   </si>
   <si>
-    <t>arrray</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/binary-tree-level-order-traversal/</t>
   </si>
   <si>
@@ -345,6 +342,42 @@
   </si>
   <si>
     <t>rotting oranges</t>
+  </si>
+  <si>
+    <t>search in rotated sorted array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-in-rotated-sorted-array/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum/</t>
+  </si>
+  <si>
+    <t>combination sum</t>
+  </si>
+  <si>
+    <t>backtracking</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutations/</t>
+  </si>
+  <si>
+    <t>permutations</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-intervals/</t>
+  </si>
+  <si>
+    <t>merge intervals</t>
+  </si>
+  <si>
+    <t>sorting</t>
+  </si>
+  <si>
+    <t>intervals</t>
+  </si>
+  <si>
+    <t>lowest common ancestor of a binary tree</t>
   </si>
 </sst>
 </file>
@@ -685,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1118,7 @@
         <v>74</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1107,7 +1140,7 @@
         <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -1118,7 +1151,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
@@ -1130,40 +1163,40 @@
         <v>32</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
         <v>81</v>
-      </c>
-      <c r="B32" t="s">
-        <v>82</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -1175,40 +1208,40 @@
         <v>2</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" t="s">
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B36" t="s">
-        <v>94</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
@@ -1217,26 +1250,26 @@
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" t="s">
         <v>99</v>
       </c>
-      <c r="B38" t="s">
-        <v>100</v>
-      </c>
       <c r="F38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
@@ -1248,12 +1281,12 @@
         <v>18</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
@@ -1268,12 +1301,12 @@
         <v>24</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -1288,7 +1321,89 @@
         <v>26</v>
       </c>
       <c r="F41" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42">
+        <v>45</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43">
+        <v>25</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>31</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding accounts merge, sort colors and time based key-value store
</commit_message>
<xml_diff>
--- a/exercises.xlsx
+++ b/exercises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="126">
   <si>
     <t>https://leetcode.com/problems/decode-ways/</t>
   </si>
@@ -377,7 +377,31 @@
     <t>intervals</t>
   </si>
   <si>
-    <t>lowest common ancestor of a binary tree</t>
+    <t>time based key-value store</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/time-based-key-value-store/</t>
+  </si>
+  <si>
+    <t>bisect</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/accounts-merge/</t>
+  </si>
+  <si>
+    <t>accounts merge</t>
+  </si>
+  <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>adjacency table</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sort-colors/</t>
+  </si>
+  <si>
+    <t>sort colors</t>
   </si>
 </sst>
 </file>
@@ -718,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,8 +1426,54 @@
       <c r="A46" t="s">
         <v>117</v>
       </c>
+      <c r="B46" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46">
+        <v>36</v>
+      </c>
       <c r="F46" t="s">
-        <v>58</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>121</v>
+      </c>
+      <c r="B47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>90</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>13</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>